<commit_message>
Added 2nd Test Method
</commit_message>
<xml_diff>
--- a/src/test/testdata/FormTestData.xlsx
+++ b/src/test/testdata/FormTestData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{6C8EF6D3-CF5E-4111-9DE4-392032D82EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{DBDA3FFA-C3DC-4AE6-AFDE-0AFF5B4BE2AC}"/>
+    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{DBDA3FFA-C3DC-4AE6-AFDE-0AFF5B4BE2AC}"/>
   </bookViews>
   <sheets>
     <sheet name="FormTestData" sheetId="1" r:id="rId1"/>
@@ -768,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4599607-550D-474C-8FC5-2B6A3C73DB3D}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>